<commit_message>
bextract data added to the training sets
</commit_message>
<xml_diff>
--- a/training-set/ratings/raw/daniel_raw.xlsx
+++ b/training-set/ratings/raw/daniel_raw.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schol\Documents\Classes\Capstone\Music\ratings\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="8148"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Intensity</t>
   </si>
@@ -95,9 +95,6 @@
     <t>better man</t>
   </si>
   <si>
-    <t>starboy - the weekend</t>
-  </si>
-  <si>
     <t>seein red</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>caroline</t>
   </si>
   <si>
-    <t>carl orff carmina bu-</t>
-  </si>
-  <si>
     <t>bad and boujee</t>
   </si>
   <si>
@@ -152,42 +146,27 @@
     <t>0:15 - 0:23</t>
   </si>
   <si>
-    <t>juju on the beat</t>
-  </si>
-  <si>
     <t>starving</t>
   </si>
   <si>
     <t>waste a moment</t>
   </si>
   <si>
-    <t>bernstein sonata for clarinate</t>
-  </si>
-  <si>
     <t>unsteady</t>
   </si>
   <si>
     <t>chain breaker</t>
   </si>
   <si>
-    <t>the weeknd - starboy</t>
-  </si>
-  <si>
     <t>lean on</t>
   </si>
   <si>
-    <t>closer - the chainsmokers</t>
-  </si>
-  <si>
     <t>vector to the heavens</t>
   </si>
   <si>
     <t>sucker for pain - lil wayne</t>
   </si>
   <si>
-    <t>let me love you - j'beeb</t>
-  </si>
-  <si>
     <t>blue aint your color</t>
   </si>
   <si>
@@ -197,21 +176,12 @@
     <t>dirty laundry</t>
   </si>
   <si>
-    <t>rockabye - clean bandit</t>
-  </si>
-  <si>
-    <t>alleluia - eric whitacre</t>
-  </si>
-  <si>
     <t>dark saint</t>
   </si>
   <si>
     <t>drake - fake love</t>
   </si>
   <si>
-    <t>in the name - martn garrix and bebe rexha</t>
-  </si>
-  <si>
     <t>0:05 - 0:19</t>
   </si>
   <si>
@@ -224,9 +194,6 @@
     <t>ophelia</t>
   </si>
   <si>
-    <t>joli garcon</t>
-  </si>
-  <si>
     <t>mortvia aqueduct</t>
   </si>
   <si>
@@ -236,9 +203,6 @@
     <t>a guy with a girl</t>
   </si>
   <si>
-    <t>back toccata and fugue in d minor</t>
-  </si>
-  <si>
     <t>look for the sliver lining</t>
   </si>
   <si>
@@ -257,9 +221,6 @@
     <t>this is what you came for</t>
   </si>
   <si>
-    <t>machine gun kelly and camila cabello - bad-</t>
-  </si>
-  <si>
     <t>king porter stomp</t>
   </si>
   <si>
@@ -269,24 +230,12 @@
     <t>light of nibel</t>
   </si>
   <si>
-    <t>don't let me down - the chainsmokers</t>
-  </si>
-  <si>
-    <t>stair way to t- glenn miller with ray erberle</t>
-  </si>
-  <si>
-    <t>machine gun kelly - bad th-</t>
-  </si>
-  <si>
     <t>dirt on my boots</t>
   </si>
   <si>
     <t>funeral ikos</t>
   </si>
   <si>
-    <t>georg friedrich handel, sonata for oboe</t>
-  </si>
-  <si>
     <t>moonglow</t>
   </si>
   <si>
@@ -321,12 +270,75 @@
   </si>
   <si>
     <t>0:04 - 0:15</t>
+  </si>
+  <si>
+    <t>starboy</t>
+  </si>
+  <si>
+    <t>carl orff carmina bu</t>
+  </si>
+  <si>
+    <t>juju on that beat</t>
+  </si>
+  <si>
+    <t>closer</t>
+  </si>
+  <si>
+    <t>sonata for clarinet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">let me love you </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alleluia </t>
+  </si>
+  <si>
+    <t>rockabye</t>
+  </si>
+  <si>
+    <t>in the name</t>
+  </si>
+  <si>
+    <t>joli gar</t>
+  </si>
+  <si>
+    <t>toccata</t>
+  </si>
+  <si>
+    <t>machine gun kelly</t>
+  </si>
+  <si>
+    <t>don't let me down</t>
+  </si>
+  <si>
+    <t>stair way to the stars</t>
+  </si>
+  <si>
+    <t>sonata for oboe</t>
+  </si>
+  <si>
+    <t>let me love you lyric</t>
+  </si>
+  <si>
+    <t>Love on the brai</t>
+  </si>
+  <si>
+    <t>starboy official</t>
+  </si>
+  <si>
+    <t>24k magic official</t>
+  </si>
+  <si>
+    <t>machine gun</t>
+  </si>
+  <si>
+    <t>closer lyric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,11 +400,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,18 +688,18 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -698,18 +710,18 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -725,7 +737,7 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -735,7 +747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -749,9 +761,9 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5">
+        <v>98</v>
+      </c>
+      <c r="F3" s="4">
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="H3" s="1">
@@ -761,7 +773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -777,11 +789,11 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -797,11 +809,11 @@
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1.5972222222222224E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -817,11 +829,11 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1.4583333333333332E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -837,11 +849,11 @@
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -857,11 +869,11 @@
       <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -877,11 +889,11 @@
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -897,11 +909,11 @@
       <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>1.3194444444444444E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -917,11 +929,11 @@
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -937,11 +949,11 @@
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -957,11 +969,11 @@
       <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -977,11 +989,11 @@
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -997,11 +1009,11 @@
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1017,11 +1029,11 @@
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1035,13 +1047,13 @@
         <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="5">
+        <v>82</v>
+      </c>
+      <c r="F17" s="4">
         <v>1.3194444444444444E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1055,13 +1067,13 @@
         <v>6</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="5">
+        <v>23</v>
+      </c>
+      <c r="F18" s="4">
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1075,13 +1087,13 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1095,13 +1107,13 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="5">
+        <v>26</v>
+      </c>
+      <c r="F20" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1115,13 +1127,13 @@
         <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="5">
+        <v>27</v>
+      </c>
+      <c r="F21" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1135,13 +1147,13 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="5">
+        <v>28</v>
+      </c>
+      <c r="F22" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1155,13 +1167,13 @@
         <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="5">
+        <v>100</v>
+      </c>
+      <c r="F23" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1175,13 +1187,13 @@
         <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="5">
+        <v>30</v>
+      </c>
+      <c r="F24" s="4">
         <v>1.1805555555555555E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1195,13 +1207,13 @@
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="5">
+        <v>31</v>
+      </c>
+      <c r="F25" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1215,13 +1227,13 @@
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="5">
+        <v>32</v>
+      </c>
+      <c r="F26" s="4">
         <v>4.1666666666666666E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1235,13 +1247,13 @@
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1255,13 +1267,13 @@
         <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="5">
+        <v>38</v>
+      </c>
+      <c r="F28" s="4">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1275,13 +1287,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1295,13 +1307,13 @@
         <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F30" s="5">
+        <v>83</v>
+      </c>
+      <c r="F30" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1315,13 +1327,13 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="5">
+        <v>84</v>
+      </c>
+      <c r="F31" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1335,13 +1347,13 @@
         <v>4</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="5">
+        <v>35</v>
+      </c>
+      <c r="F32" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1355,13 +1367,13 @@
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="5">
+        <v>36</v>
+      </c>
+      <c r="F33" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1377,11 +1389,11 @@
       <c r="E34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="4">
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1395,13 +1407,13 @@
         <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="5">
+        <v>40</v>
+      </c>
+      <c r="F35" s="4">
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1415,13 +1427,13 @@
         <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="5">
+        <v>85</v>
+      </c>
+      <c r="F36" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1435,13 +1447,13 @@
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="5">
+        <v>41</v>
+      </c>
+      <c r="F37" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1455,13 +1467,13 @@
         <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="5">
+        <v>86</v>
+      </c>
+      <c r="F38" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1475,13 +1487,13 @@
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="5">
+        <v>42</v>
+      </c>
+      <c r="F39" s="4">
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1495,13 +1507,13 @@
         <v>6</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="5">
+        <v>43</v>
+      </c>
+      <c r="F40" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1515,13 +1527,13 @@
         <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F41" s="5">
+        <v>99</v>
+      </c>
+      <c r="F41" s="4">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1535,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="5">
+        <v>44</v>
+      </c>
+      <c r="F42" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1555,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="5">
+        <v>102</v>
+      </c>
+      <c r="F43" s="4">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1575,13 +1587,13 @@
         <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F44" s="5">
+        <v>45</v>
+      </c>
+      <c r="F44" s="4">
         <v>1.5277777777777777E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1595,13 +1607,13 @@
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F45" s="5">
+        <v>46</v>
+      </c>
+      <c r="F45" s="4">
         <v>2.2916666666666669E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1615,13 +1627,13 @@
         <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" s="5">
+        <v>87</v>
+      </c>
+      <c r="F46" s="4">
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1635,13 +1647,13 @@
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F47" s="5">
+        <v>47</v>
+      </c>
+      <c r="F47" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1655,13 +1667,13 @@
         <v>6</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="5">
+        <v>48</v>
+      </c>
+      <c r="F48" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1675,13 +1687,13 @@
         <v>7</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1695,13 +1707,13 @@
         <v>7</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" s="5">
+        <v>89</v>
+      </c>
+      <c r="F50" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1715,13 +1727,13 @@
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="F51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1735,13 +1747,13 @@
         <v>9</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F52" s="5">
+        <v>50</v>
+      </c>
+      <c r="F52" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1755,13 +1767,13 @@
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F53" s="5">
+        <v>51</v>
+      </c>
+      <c r="F53" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1775,13 +1787,13 @@
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1795,13 +1807,13 @@
         <v>8</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F55" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1815,13 +1827,13 @@
         <v>8</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F56" s="5">
+        <v>91</v>
+      </c>
+      <c r="F56" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1835,13 +1847,13 @@
         <v>8</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1855,13 +1867,13 @@
         <v>7</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F58" s="5">
+        <v>57</v>
+      </c>
+      <c r="F58" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -1875,13 +1887,13 @@
         <v>9</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F59" s="5">
+        <v>58</v>
+      </c>
+      <c r="F59" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -1895,13 +1907,13 @@
         <v>7</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="F60" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -1915,13 +1927,13 @@
         <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F61" s="5">
+        <v>59</v>
+      </c>
+      <c r="F61" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -1935,13 +1947,13 @@
         <v>7</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -1955,13 +1967,13 @@
         <v>8</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F63" s="5">
+        <v>97</v>
+      </c>
+      <c r="F63" s="4">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1975,13 +1987,13 @@
         <v>8</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F64" s="5">
+        <v>61</v>
+      </c>
+      <c r="F64" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -1995,13 +2007,13 @@
         <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F65" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2015,13 +2027,13 @@
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F66" s="5">
+        <v>63</v>
+      </c>
+      <c r="F66" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2035,13 +2047,13 @@
         <v>7</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F67" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2055,13 +2067,13 @@
         <v>7</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F68" s="5">
+        <v>101</v>
+      </c>
+      <c r="F68" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2075,13 +2087,13 @@
         <v>8</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F69" s="5">
+        <v>65</v>
+      </c>
+      <c r="F69" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2095,13 +2107,13 @@
         <v>7</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="F70" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2115,13 +2127,13 @@
         <v>8</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F71" s="5">
+        <v>79</v>
+      </c>
+      <c r="F71" s="4">
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2135,13 +2147,13 @@
         <v>9</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F72" s="5">
+        <v>67</v>
+      </c>
+      <c r="F72" s="4">
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2155,13 +2167,13 @@
         <v>7</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F73" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2175,13 +2187,13 @@
         <v>6</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F74" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2195,13 +2207,13 @@
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F75" s="5">
+        <v>29</v>
+      </c>
+      <c r="F75" s="4">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2215,13 +2227,13 @@
         <v>8</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F76" s="5">
+        <v>93</v>
+      </c>
+      <c r="F76" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2235,13 +2247,13 @@
         <v>8</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F77" s="5">
+        <v>68</v>
+      </c>
+      <c r="F77" s="4">
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2255,13 +2267,13 @@
         <v>7</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F78" s="5">
+        <v>69</v>
+      </c>
+      <c r="F78" s="4">
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2275,13 +2287,13 @@
         <v>8</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F79" s="5">
+        <v>96</v>
+      </c>
+      <c r="F79" s="4">
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2295,13 +2307,13 @@
         <v>8</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F80" s="5">
+        <v>70</v>
+      </c>
+      <c r="F80" s="4">
         <v>1.1805555555555555E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2315,9 +2327,9 @@
         <v>9</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F81" s="5">
+        <v>71</v>
+      </c>
+      <c r="F81" s="4">
         <v>1.1111111111111112E-2</v>
       </c>
     </row>

</xml_diff>